<commit_message>
upload vehicle sheet api now throws error
</commit_message>
<xml_diff>
--- a/uploads/VehicleRegistry.xlsx
+++ b/uploads/VehicleRegistry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tinduvo/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94D2019-C981-DD43-B2EF-E39D726F3015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE18A35-DBB9-6943-91EC-D938C04CF894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="560" windowWidth="25240" windowHeight="17440" xr2:uid="{966CC084-EDED-6745-8CAC-6017D5A4AF3A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>License plate</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>car</t>
+  </si>
+  <si>
+    <t>Owner phone number</t>
+  </si>
+  <si>
+    <t>09123456789</t>
+  </si>
+  <si>
+    <t>09123456788</t>
+  </si>
+  <si>
+    <t>09123456787</t>
   </si>
 </sst>
 </file>
@@ -264,8 +276,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{812754E0-B3FB-1E48-9F76-92C6239D04FA}">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -597,12 +609,13 @@
     <col min="11" max="11" width="20.6640625" customWidth="1"/>
     <col min="13" max="13" width="11.83203125" customWidth="1"/>
     <col min="14" max="14" width="13.6640625" customWidth="1"/>
-    <col min="17" max="17" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="21" customWidth="1"/>
     <col min="18" max="18" width="12.6640625" customWidth="1"/>
     <col min="19" max="19" width="13.6640625" customWidth="1"/>
+    <col min="21" max="21" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -651,26 +664,27 @@
       <c r="P1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>52</v>
       </c>
@@ -689,7 +703,7 @@
       <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>45272</v>
       </c>
       <c r="I2" s="1">
@@ -717,7 +731,7 @@
         <v>10000</v>
       </c>
       <c r="Q2" s="1">
-        <v>1234567890</v>
+        <v>111111111111</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>45</v>
@@ -725,14 +739,17 @@
       <c r="S2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="4">
         <v>33219</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -754,7 +771,7 @@
       <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>45273</v>
       </c>
       <c r="I3" s="1">
@@ -782,7 +799,7 @@
         <v>10000</v>
       </c>
       <c r="Q3" s="1">
-        <v>1234567892</v>
+        <v>111111111112</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>46</v>
@@ -790,14 +807,17 @@
       <c r="S3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T3" s="5">
+      <c r="T3" s="4">
         <v>33220</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -819,7 +839,7 @@
       <c r="G4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>45274</v>
       </c>
       <c r="I4" s="1">
@@ -847,7 +867,7 @@
         <v>10000</v>
       </c>
       <c r="Q4" s="1">
-        <v>1234567890</v>
+        <v>111111111111</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>45</v>
@@ -855,14 +875,17 @@
       <c r="S4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="5">
+      <c r="T4" s="4">
         <v>33221</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -884,7 +907,7 @@
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>45275</v>
       </c>
       <c r="I5" s="1">
@@ -912,7 +935,7 @@
         <v>10000</v>
       </c>
       <c r="Q5" s="1">
-        <v>1234567891</v>
+        <v>111111111112</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>46</v>
@@ -920,14 +943,17 @@
       <c r="S5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T5" s="5">
+      <c r="T5" s="4">
         <v>33222</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="V5" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -949,7 +975,7 @@
       <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>45276</v>
       </c>
       <c r="I6" s="1">
@@ -977,7 +1003,7 @@
         <v>10000</v>
       </c>
       <c r="Q6" s="1">
-        <v>1234567890</v>
+        <v>111111111111</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>45</v>
@@ -985,14 +1011,17 @@
       <c r="S6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="5">
+      <c r="T6" s="4">
         <v>33223</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -1014,7 +1043,7 @@
       <c r="G7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>45277</v>
       </c>
       <c r="I7" s="1">
@@ -1042,7 +1071,7 @@
         <v>10000</v>
       </c>
       <c r="Q7" s="1">
-        <v>1234567890</v>
+        <v>111111111112</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>46</v>
@@ -1050,14 +1079,17 @@
       <c r="S7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="4">
         <v>33224</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="U7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V7" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1079,7 +1111,7 @@
       <c r="G8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>45278</v>
       </c>
       <c r="I8" s="1">
@@ -1107,7 +1139,7 @@
         <v>10000</v>
       </c>
       <c r="Q8" s="1">
-        <v>1234567890</v>
+        <v>111111111111</v>
       </c>
       <c r="R8" s="1" t="s">
         <v>45</v>
@@ -1115,10 +1147,13 @@
       <c r="S8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T8" s="5">
+      <c r="T8" s="4">
         <v>33225</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1126,5 +1161,8 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="U2 U6:U8 U4 U3 U5" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>